<commit_message>
Add ApDocument model test
</commit_message>
<xml_diff>
--- a/apflow/tests/data/test_data.xlsx
+++ b/apflow/tests/data/test_data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -165,22 +165,43 @@
     <t xml:space="preserve">Company 1</t>
   </si>
   <si>
+    <t xml:space="preserve">"111222333"</t>
+  </si>
+  <si>
     <t xml:space="preserve">Company 2</t>
   </si>
   <si>
+    <t xml:space="preserve">"111222334"</t>
+  </si>
+  <si>
     <t xml:space="preserve">Company 3</t>
   </si>
   <si>
+    <t xml:space="preserve">"111222335"</t>
+  </si>
+  <si>
     <t xml:space="preserve">Company 4</t>
   </si>
   <si>
+    <t xml:space="preserve">"111222336"</t>
+  </si>
+  <si>
     <t xml:space="preserve">Company 5</t>
   </si>
   <si>
+    <t xml:space="preserve">"111222337"</t>
+  </si>
+  <si>
     <t xml:space="preserve">Company 6</t>
   </si>
   <si>
+    <t xml:space="preserve">"111222338"</t>
+  </si>
+  <si>
     <t xml:space="preserve">Company 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"111222339"</t>
   </si>
 </sst>
 </file>
@@ -284,7 +305,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C5:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -415,7 +436,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="C5:D8 B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -528,7 +549,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N17" activeCellId="0" sqref="N17"/>
+      <selection pane="topLeft" activeCell="N17" activeCellId="1" sqref="C5:D8 N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -622,7 +643,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="C5:D8 B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -806,7 +827,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="C5:D8 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -931,17 +952,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -951,61 +972,109 @@
       <c r="B1" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>111222333</v>
+      <c r="B2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>111222334</v>
+        <v>47</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>111222335</v>
+        <v>49</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>111222336</v>
+        <v>51</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>111222337</v>
+        <v>53</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="1" t="n">
-        <v>111222338</v>
+        <v>55</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="1" t="n">
-        <v>111222339</v>
+        <v>57</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Forgot to add some files
</commit_message>
<xml_diff>
--- a/apflow/tests/data/test_data.xlsx
+++ b/apflow/tests/data/test_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,7 @@
     <sheet name="company_units" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="employees" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="counterparties" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="counterparty_notes" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="68">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -165,51 +166,79 @@
     <t xml:space="preserve">Company 1</t>
   </si>
   <si>
-    <t xml:space="preserve">"111222333"</t>
+    <t xml:space="preserve">111222333</t>
   </si>
   <si>
     <t xml:space="preserve">Company 2</t>
   </si>
   <si>
-    <t xml:space="preserve">"111222334"</t>
+    <t xml:space="preserve">111222334</t>
   </si>
   <si>
     <t xml:space="preserve">Company 3</t>
   </si>
   <si>
-    <t xml:space="preserve">"111222335"</t>
+    <t xml:space="preserve">111222335</t>
   </si>
   <si>
     <t xml:space="preserve">Company 4</t>
   </si>
   <si>
-    <t xml:space="preserve">"111222336"</t>
+    <t xml:space="preserve">111222336</t>
   </si>
   <si>
     <t xml:space="preserve">Company 5</t>
   </si>
   <si>
-    <t xml:space="preserve">"111222337"</t>
+    <t xml:space="preserve">111222337</t>
   </si>
   <si>
     <t xml:space="preserve">Company 6</t>
   </si>
   <si>
-    <t xml:space="preserve">"111222338"</t>
+    <t xml:space="preserve">111222338</t>
   </si>
   <si>
     <t xml:space="preserve">Company 7</t>
   </si>
   <si>
-    <t xml:space="preserve">"111222339"</t>
+    <t xml:space="preserve">111222339</t>
+  </si>
+  <si>
+    <t xml:space="preserve">counterparty_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note 2 – 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note 2 – 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note 2 – 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note 3 – 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -276,12 +305,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -305,14 +342,15 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C5:D8"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -436,13 +474,15 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="C5:D8 B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -549,10 +589,13 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N17" activeCellId="1" sqref="C5:D8 N17"/>
+      <selection pane="topLeft" activeCell="N17" activeCellId="0" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -643,12 +686,14 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="C5:D8 B4"/>
+      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -827,13 +872,15 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="C5:D8 E1"/>
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -954,23 +1001,166 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5:D8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0561224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5357142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.50510204081633"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>3</v>
@@ -980,11 +1170,11 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>46</v>
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>61</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
@@ -994,11 +1184,11 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>48</v>
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>62</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1</v>
@@ -1008,11 +1198,11 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>50</v>
+      <c r="A4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>63</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1</v>
@@ -1022,11 +1212,11 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>52</v>
+      <c r="A5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>64</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1</v>
@@ -1036,11 +1226,11 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>54</v>
+      <c r="A6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>65</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>
@@ -1050,11 +1240,11 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>56</v>
+      <c r="A7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
@@ -1064,11 +1254,11 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>58</v>
+      <c r="A8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>67</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Add some sample data
</commit_message>
<xml_diff>
--- a/apflow/tests/data/test_data.xlsx
+++ b/apflow/tests/data/test_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,6 +17,7 @@
     <sheet name="counterparty_notes" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="cost_accounts" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="ap_documents" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="ap_document_cd" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="149">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -45,34 +46,34 @@
     <t xml:space="preserve">updated_by</t>
   </si>
   <si>
-    <t xml:space="preserve">bnm_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bnm_name@local.host</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b1_man_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b1_man_name@local.host</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b1_acc_name1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b1_acc_name1@local.host</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b1_om_1_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b1_om_1_name@local.host</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b2_acc_name1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b2_acc_name1@local.host</t>
+    <t xml:space="preserve">a_bnm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a_bnm@local.host</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b_b1_bman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b_b1_bman@local.host</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c_b1_acc1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c_b1_acc1@local.host</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c_b1_om1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c_b1_om1@local.host</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c_b2_acc1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c_b2_acc1@local.host</t>
   </si>
   <si>
     <t xml:space="preserve">name</t>
@@ -81,25 +82,25 @@
     <t xml:space="preserve">description</t>
   </si>
   <si>
-    <t xml:space="preserve">bnm_role</t>
+    <t xml:space="preserve">role_bnm</t>
   </si>
   <si>
     <t xml:space="preserve">Branch network manager</t>
   </si>
   <si>
-    <t xml:space="preserve">bm_role</t>
+    <t xml:space="preserve">role_bm</t>
   </si>
   <si>
     <t xml:space="preserve">Branch manager</t>
   </si>
   <si>
-    <t xml:space="preserve">b_acc_role</t>
+    <t xml:space="preserve">role_b_acc</t>
   </si>
   <si>
     <t xml:space="preserve">Branch accountant</t>
   </si>
   <si>
-    <t xml:space="preserve">b_om_role</t>
+    <t xml:space="preserve">role_b_om</t>
   </si>
   <si>
     <t xml:space="preserve">Office manager</t>
@@ -150,16 +151,19 @@
     <t xml:space="preserve">company_unit_id</t>
   </si>
   <si>
-    <t xml:space="preserve">bnm_full_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b1_man_full_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b1_acc_full_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b1_om1_full_name</t>
+    <t xml:space="preserve">A_bm_full_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1_man_full_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1_acc1_full_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1_om1_full_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B2_acc1_full_name</t>
   </si>
   <si>
     <t xml:space="preserve">eik_egn</t>
@@ -207,6 +211,84 @@
     <t xml:space="preserve">111222339</t>
   </si>
   <si>
+    <t xml:space="preserve">Company 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111222340</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111222341</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111222342</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111222343</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111222344</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111222345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111222346</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111222347</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111222348</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111222349</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111222350</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111222351</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111222352</t>
+  </si>
+  <si>
     <t xml:space="preserve">counterparty_id</t>
   </si>
   <si>
@@ -249,6 +331,18 @@
     <t xml:space="preserve">Р-ди за материали 2</t>
   </si>
   <si>
+    <t xml:space="preserve">6010000003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Р-ди за материали 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6010000004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Р-ди за материали 4</t>
+  </si>
+  <si>
     <t xml:space="preserve">6020000001</t>
   </si>
   <si>
@@ -261,6 +355,18 @@
     <t xml:space="preserve">Р-ди външни услуги 2</t>
   </si>
   <si>
+    <t xml:space="preserve">6020000003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Р-ди външни услуги 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6020000004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Р-ди външни услуги 4</t>
+  </si>
+  <si>
     <t xml:space="preserve">6090000001</t>
   </si>
   <si>
@@ -273,6 +379,9 @@
     <t xml:space="preserve">Други р-ди – командировки – пътни</t>
   </si>
   <si>
+    <t xml:space="preserve">init_unit_id</t>
+  </si>
+  <si>
     <t xml:space="preserve">doc_number</t>
   </si>
   <si>
@@ -325,6 +434,48 @@
   </si>
   <si>
     <t xml:space="preserve">pending_bna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">501</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Info 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add info 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">level_acc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">502</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Info 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add info 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">503</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Info 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add info 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pending_acc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apdoc_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost_account_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amount</t>
   </si>
 </sst>
 </file>
@@ -442,7 +593,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="1" sqref="J2:K3 C8"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -559,6 +710,236 @@
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.7704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1836734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>300.5</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>25.86</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>100.2</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>500.1</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>450</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>450.69</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -574,7 +955,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="J2:K3 B6"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -686,10 +1067,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N17" activeCellId="1" sqref="J2:K3 N17"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -764,6 +1145,20 @@
         <v>1</v>
       </c>
       <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -786,7 +1181,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D33" activeCellId="1" sqref="J2:K3 D33"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -969,10 +1364,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="1" sqref="J2:K3 C24"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1080,6 +1475,26 @@
         <v>1</v>
       </c>
       <c r="F5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1099,14 +1514,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="J2:K3 D1"/>
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5867346938776"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.6887755102041"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.36734693877551"/>
   </cols>
@@ -1116,7 +1532,7 @@
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>3</v>
@@ -1127,10 +1543,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
@@ -1141,10 +1557,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1</v>
@@ -1155,10 +1571,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1</v>
@@ -1169,10 +1585,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1</v>
@@ -1183,10 +1599,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>
@@ -1197,10 +1613,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
@@ -1211,15 +1627,197 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1242,7 +1840,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="J2:K3 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1255,10 +1853,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>3</v>
@@ -1272,7 +1870,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
@@ -1286,7 +1884,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1</v>
@@ -1300,7 +1898,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1</v>
@@ -1314,7 +1912,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1</v>
@@ -1328,7 +1926,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>
@@ -1342,7 +1940,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
@@ -1356,7 +1954,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1</v>
@@ -1381,22 +1979,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="J2:K3 C1"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9336734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.5357142857143"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>15</v>
@@ -1410,10 +2008,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
@@ -1424,10 +2022,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1</v>
@@ -1438,10 +2036,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1</v>
@@ -1452,10 +2050,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1</v>
@@ -1466,10 +2064,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>
@@ -1480,15 +2078,71 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1508,52 +2162,56 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2:K3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1836734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>118</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>85</v>
+        <v>120</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>86</v>
+        <v>121</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>87</v>
+        <v>122</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>88</v>
+        <v>123</v>
       </c>
       <c r="J1" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="K1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="L1" s="0" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1561,70 +2219,190 @@
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" s="4" t="n">
+      <c r="B2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="4" t="n">
         <v>43191</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="E2" s="0" t="n">
         <v>500.5</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>90</v>
-      </c>
       <c r="F2" s="0" t="s">
-        <v>91</v>
+        <v>126</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>92</v>
+        <v>127</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>93</v>
+        <v>128</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>1</v>
+        <v>129</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>130</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="4" t="n">
         <v>43200</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="E3" s="0" t="n">
         <v>25.86</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>96</v>
-      </c>
       <c r="F3" s="0" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>92</v>
+        <v>133</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>93</v>
+        <v>128</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>1</v>
+        <v>129</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>134</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>43160</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>100.2</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>43160</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>5000.1</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>43160</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1500.69</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>